<commit_message>
maybe need to add filter for none values
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonea\excel-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OnTrac\python_Ontrac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1FFE82-7AC7-40AD-8142-49F7B7D9736F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFC90B4-7606-4E63-B497-EB6BADE9A9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="10860" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="8895" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,8 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,205 +535,209 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="3" max="6" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>